<commit_message>
Finished moving configuration to excel
</commit_message>
<xml_diff>
--- a/deap/tests/testing_zdt1.xlsx
+++ b/deap/tests/testing_zdt1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
   <si>
     <t>Yes</t>
   </si>
@@ -248,6 +248,54 @@
   </si>
   <si>
     <t>mj_random_jump</t>
+  </si>
+  <si>
+    <t>mj_zdt1_decimal</t>
+  </si>
+  <si>
+    <t>tools</t>
+  </si>
+  <si>
+    <t>selNSGA2</t>
+  </si>
+  <si>
+    <t>mj_evaluators</t>
+  </si>
+  <si>
+    <t>mj_algorithms</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>mutate</t>
+  </si>
+  <si>
+    <t>mj_operators</t>
+  </si>
+  <si>
+    <t>selTournamentDCD</t>
+  </si>
+  <si>
+    <t>Probability crossover</t>
+  </si>
+  <si>
+    <t>mate</t>
+  </si>
+  <si>
+    <t>Probability flip allele</t>
+  </si>
+  <si>
+    <t>Jump size</t>
+  </si>
+  <si>
+    <t>Probability mutation</t>
   </si>
 </sst>
 </file>
@@ -684,31 +732,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B1">
+      <c r="B2">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4">
+        <v>0.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6">
         <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -718,65 +827,101 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
       <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Retrieve population from database (reload) Progress
</commit_message>
<xml_diff>
--- a/deap/tests/testing_zdt1.xlsx
+++ b/deap/tests/testing_zdt1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="17490" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="3" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
   <si>
     <t>Yes</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>Probability mutation</t>
+  </si>
+  <si>
+    <t>continue_run</t>
   </si>
 </sst>
 </file>
@@ -670,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +726,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -734,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +781,7 @@
         <v>12</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="C3" t="s">
         <v>65</v>

</xml_diff>